<commit_message>
updated Report script of scenario 6
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioSix201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioSix201718.xlsx
@@ -4,22 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2376" windowWidth="9552" windowHeight="3564" firstSheet="3" activeTab="5"/>
+    <workbookView activeTab="5" firstSheet="3" windowHeight="3564" windowWidth="9552" xWindow="0" yWindow="2376"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM12" sheetId="61" r:id="rId3"/>
-    <sheet name="ProcessPayrollForMarch" sheetId="60" r:id="rId4"/>
-    <sheet name="ProcessFinalPayrollForMarch" sheetId="59" r:id="rId5"/>
-    <sheet name="TestMarchReports" sheetId="44" r:id="rId6"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM12" r:id="rId3" sheetId="61"/>
+    <sheet name="ProcessPayrollForMarch" r:id="rId4" sheetId="60"/>
+    <sheet name="ProcessFinalPayrollForMarch" r:id="rId5" sheetId="59"/>
+    <sheet name="TestMarchReports" r:id="rId6" sheetId="44"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="65">
   <si>
     <t>TC</t>
   </si>
@@ -220,6 +220,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -279,51 +280,51 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="2">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -337,10 +338,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -498,7 +499,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -507,13 +508,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -523,7 +524,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -532,7 +533,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -541,7 +542,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -551,12 +552,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -587,7 +588,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -606,7 +607,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -618,7 +619,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -627,10 +628,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.77734375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -732,12 +733,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -746,19 +747,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="29.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="22.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.6640625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.21875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="6.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="8.109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="29.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="6.21875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -802,7 +803,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="30" r="2" s="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>46</v>
       </c>
@@ -842,13 +843,13 @@
       <c r="O2" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -857,9 +858,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -891,7 +892,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="40.799999999999997" r="2" s="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
@@ -915,12 +916,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -929,13 +930,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.21875" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" customWidth="1"/>
-    <col min="7" max="7" width="34.33203125" customWidth="1"/>
-    <col min="8" max="8" width="38.109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="27.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -982,7 +983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>24</v>
       </c>
@@ -1024,15 +1025,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a1Fb0000007Xdp2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000007Xdp2" r:id="rId2" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -1041,14 +1042,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="45.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.77734375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -1095,7 +1096,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>24</v>
       </c>
@@ -1137,15 +1138,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a1Fb0000007Xdp2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000007Xdp2" r:id="rId2" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1154,20 +1155,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.21875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="24.77734375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="41.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.21875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="48.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row ht="28.8" r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1220,7 +1221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>24</v>
       </c>
@@ -1269,9 +1270,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a1Fb0000007Xdp2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a1Fb0000007Xdp2" r:id="rId2" ref="E2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Page Navigation logic code checkin- RTI Scenarios from 3 to 7
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioSix201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioSix201718.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="5" firstSheet="3" windowHeight="3576" windowWidth="9552" xWindow="0" yWindow="2376"/>
+    <workbookView windowHeight="3570" windowWidth="9555" xWindow="0" yWindow="2370"/>
   </bookViews>
   <sheets>
     <sheet name="first" r:id="rId1" sheetId="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="65">
   <si>
     <t>TC</t>
   </si>
@@ -102,9 +107,6 @@
     <t>TestRemarkRowNumOfTestResultFile</t>
   </si>
   <si>
-    <t>ResetEmployeeData</t>
-  </si>
-  <si>
     <t>AddressFirstLine</t>
   </si>
   <si>
@@ -214,12 +216,15 @@
   </si>
   <si>
     <t>HMRCS6_Payroll</t>
+  </si>
+  <si>
+    <t>ResetEmployeeData12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -379,7 +384,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -412,9 +417,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,6 +469,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -625,15 +664,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
@@ -653,7 +692,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>23</v>
@@ -667,7 +706,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>23</v>
@@ -681,7 +720,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>23</v>
@@ -695,7 +734,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>23</v>
@@ -709,7 +748,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
@@ -723,7 +762,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>23</v>
@@ -748,53 +787,53 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="8.109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="29.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="9.6640625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="6.33203125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="6.44140625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="29.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
@@ -808,28 +847,28 @@
     </row>
     <row customFormat="1" customHeight="1" ht="30" r="2" s="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>48</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>49</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>7</v>
@@ -859,14 +898,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -874,16 +913,16 @@
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -895,21 +934,21 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="40.950000000000003" r="2" s="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="40.9" r="2" s="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>8</v>
@@ -931,18 +970,18 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="36.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="38.109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="38.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -986,30 +1025,30 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>21</v>
@@ -1018,7 +1057,7 @@
         <v>19</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -1043,19 +1082,19 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="38.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.33203125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="28.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="34.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="45.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="28.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="45.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1099,39 +1138,39 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="H2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -1151,23 +1190,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="41.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.140625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="31.0" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="48.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.33203125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="11" max="14" customWidth="true" width="24.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="11" max="14" customWidth="true" width="24.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row ht="30" r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1223,48 +1262,48 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
HTML Output files checkin
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioSix201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioSix201718.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="3570" windowWidth="9555" xWindow="0" yWindow="2370"/>
+    <workbookView activeTab="5" firstSheet="3" windowHeight="3570" windowWidth="9555" xWindow="0" yWindow="2370"/>
   </bookViews>
   <sheets>
     <sheet name="first" r:id="rId1" sheetId="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="65">
   <si>
     <t>TC</t>
   </si>
@@ -155,9 +155,6 @@
     <t>UpdteTaxCodeAndAnualSalaryM12</t>
   </si>
   <si>
-    <t>DO NOT TOUCH AUTOMATION HMRC RECOGNITION EMPLOYEE 106</t>
-  </si>
-  <si>
     <t>03/01/2018</t>
   </si>
   <si>
@@ -219,6 +216,9 @@
   </si>
   <si>
     <t>ResetEmployeeData12</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION HMRC RECOGNITION EMPLOYEE 6</t>
   </si>
 </sst>
 </file>
@@ -664,7 +664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -706,7 +706,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>23</v>
@@ -784,7 +784,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,28 +847,28 @@
     </row>
     <row customFormat="1" customHeight="1" ht="30" r="2" s="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>32</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>7</v>
@@ -895,7 +895,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,16 +913,16 @@
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -936,19 +936,19 @@
     </row>
     <row customFormat="1" customHeight="1" ht="40.9" r="2" s="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>8</v>
@@ -967,7 +967,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,25 +1027,25 @@
     </row>
     <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>37</v>
@@ -1057,7 +1057,7 @@
         <v>19</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -1079,7 +1079,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,37 +1140,37 @@
     </row>
     <row customFormat="1" customHeight="1" ht="42.6" r="2" s="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>37</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>4</v>
@@ -1190,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,46 +1264,46 @@
     </row>
     <row customFormat="1" customHeight="1" ht="45.6" r="2" s="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>37</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>4</v>

</xml_diff>